<commit_message>
Finished Ordering and stock control
</commit_message>
<xml_diff>
--- a/RemoteLabs_supervisor_PCB/BOM_Still to orderL.xlsx
+++ b/RemoteLabs_supervisor_PCB/BOM_Still to orderL.xlsx
@@ -1317,9 +1317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1724,7 @@
       <c r="F23" t="s">
         <v>59</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="7" t="s">
         <v>61</v>
       </c>
       <c r="H23" t="s">
@@ -1953,8 +1953,9 @@
     <hyperlink ref="G25" r:id="rId7"/>
     <hyperlink ref="G26" r:id="rId8"/>
     <hyperlink ref="G22" r:id="rId9"/>
+    <hyperlink ref="G23" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>